<commit_message>
se agrego el Join a la tabla
</commit_message>
<xml_diff>
--- a/ENVIPE_2024.xlsx
+++ b/ENVIPE_2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\misDocs\2025\INEGI\QGIS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{027C554D-9C5E-4032-A648-E61CBD7DEEB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D7FEAE4-90FE-49B3-888A-DB968E7CB599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30750" yWindow="1950" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{6DBC8393-4D26-4DC0-AF33-FAB7DC3BCE77}"/>
+    <workbookView xWindow="38070" yWindow="345" windowWidth="17370" windowHeight="14475" xr2:uid="{6DBC8393-4D26-4DC0-AF33-FAB7DC3BCE77}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -42,9 +42,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="24">
   <si>
-    <t>CVE_ENT</t>
-  </si>
-  <si>
     <t>ENVIPE_2024</t>
   </si>
   <si>
@@ -112,6 +109,9 @@
   </si>
   <si>
     <t>Temporalidad</t>
+  </si>
+  <si>
+    <t>CVEGEO</t>
   </si>
 </sst>
 </file>
@@ -497,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC6582CB-5724-4CE7-8563-0E4522435A6A}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,13 +509,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -523,7 +523,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -534,7 +534,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -545,7 +545,7 @@
         <v>15</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -556,7 +556,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -567,7 +567,7 @@
         <v>23</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -578,7 +578,7 @@
         <v>27</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -589,7 +589,7 @@
         <v>32</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -597,10 +597,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -608,10 +608,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -619,10 +619,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -633,7 +633,7 @@
         <v>16</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -644,7 +644,7 @@
         <v>21</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -655,7 +655,7 @@
         <v>30</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -663,10 +663,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C15">
         <v>3</v>
@@ -677,7 +677,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C16">
         <v>3</v>
@@ -688,7 +688,7 @@
         <v>19</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17">
         <v>3</v>
@@ -699,7 +699,7 @@
         <v>24</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C18">
         <v>3</v>
@@ -710,7 +710,7 @@
         <v>26</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C19">
         <v>3</v>
@@ -721,7 +721,7 @@
         <v>28</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C20">
         <v>3</v>
@@ -729,10 +729,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="C21">
         <v>4</v>
@@ -740,10 +740,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C22">
         <v>4</v>
@@ -754,7 +754,7 @@
         <v>13</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C23">
         <v>4</v>
@@ -765,7 +765,7 @@
         <v>20</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C24">
         <v>4</v>
@@ -776,7 +776,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C25">
         <v>4</v>
@@ -787,7 +787,7 @@
         <v>29</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C26">
         <v>4</v>
@@ -795,10 +795,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C27">
         <v>5</v>
@@ -806,10 +806,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C28">
         <v>5</v>
@@ -817,10 +817,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C29">
         <v>5</v>
@@ -831,7 +831,7 @@
         <v>10</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C30">
         <v>5</v>
@@ -842,7 +842,7 @@
         <v>18</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C31">
         <v>5</v>
@@ -853,7 +853,7 @@
         <v>22</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C32">
         <v>5</v>
@@ -864,7 +864,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C33">
         <v>5</v>
@@ -884,7 +884,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26803F04-B8E9-468C-AE87-B46FF0510F7B}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -896,23 +896,23 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3">
         <v>2024</v>
@@ -920,10 +920,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>